<commit_message>
Added the unimodal loss with binomial
</commit_message>
<xml_diff>
--- a/logs_regression.xlsx
+++ b/logs_regression.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="405">
   <si>
     <t>Date</t>
   </si>
@@ -1225,28 +1225,13 @@
     <t>February08  04:13:28</t>
   </si>
   <si>
-    <t>February15  16:26:07</t>
+    <t>February15  17:07:01</t>
   </si>
   <si>
     <t>house_16H</t>
   </si>
   <si>
     <t>False</t>
-  </si>
-  <si>
-    <t>February15  16:27:03</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>February15  16:27:19</t>
-  </si>
-  <si>
-    <t>February15  16:31:55</t>
-  </si>
-  <si>
-    <t>February15  16:32:06</t>
   </si>
 </sst>
 </file>
@@ -1633,7 +1618,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:AC366"/>
+  <dimension ref="A1:AC362"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
@@ -33807,363 +33792,64 @@
         <v>404</v>
       </c>
       <c r="J362" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="K362" t="n">
-        <v>4.166119006453862e-05</v>
+        <v>0.0007410549040639132</v>
       </c>
       <c r="L362" t="n">
-        <v>4.169410887755669e-05</v>
+        <v>0.0007480334415312291</v>
       </c>
       <c r="M362" t="n">
-        <v>0.1009491413836616</v>
+        <v>0.240302847424151</v>
       </c>
       <c r="N362" t="n">
-        <v>0.1009657594381036</v>
+        <v>0.2467076382791923</v>
       </c>
       <c r="O362" t="n">
-        <v>3.268258929715837</v>
+        <v>1.957845652342896</v>
       </c>
       <c r="P362" t="n">
-        <v>3.030681561746366</v>
+        <v>1.940793986848018</v>
       </c>
       <c r="Q362" t="n">
-        <v>2.724858726065727</v>
+        <v>1.440335765622428</v>
       </c>
       <c r="R362" t="n">
-        <v>2.582309043020193</v>
+        <v>1.42208077260755</v>
       </c>
       <c r="S362" t="n">
-        <v>0.2910517364349591</v>
+        <v>0.6140889888626763</v>
       </c>
       <c r="T362" t="n">
-        <v>0.2947761194029851</v>
+        <v>0.6165496049165935</v>
       </c>
       <c r="U362" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="V362" t="n">
-        <v>0.1009491413836616</v>
+        <v>0.2451857135019476</v>
       </c>
       <c r="W362" t="n">
-        <v>0.1009657594381036</v>
+        <v>0.2451857135019476</v>
       </c>
       <c r="X362" t="n">
-        <v>3.268258929715837</v>
+        <v>1.945730484986625</v>
       </c>
       <c r="Y362" t="n">
-        <v>3.030681561746366</v>
+        <v>1.945730484986625</v>
       </c>
       <c r="Z362" t="n">
-        <v>2.724858726065727</v>
+        <v>1.428704668897789</v>
       </c>
       <c r="AA362" t="n">
-        <v>2.582309043020193</v>
+        <v>1.428704668897789</v>
       </c>
       <c r="AB362" t="n">
-        <v>0.2910517364349591</v>
+        <v>0.6146924891644264</v>
       </c>
       <c r="AC362" t="n">
-        <v>0.2947761194029851</v>
-      </c>
-    </row>
-    <row r="363" spans="1:29">
-      <c r="A363" t="s">
-        <v>405</v>
-      </c>
-      <c r="B363" t="s">
-        <v>403</v>
-      </c>
-      <c r="C363" t="s">
-        <v>27</v>
-      </c>
-      <c r="D363" t="s">
-        <v>312</v>
-      </c>
-      <c r="E363" t="s">
-        <v>29</v>
-      </c>
-      <c r="F363" t="s">
-        <v>51</v>
-      </c>
-      <c r="G363" t="s">
-        <v>31</v>
-      </c>
-      <c r="H363" t="s">
-        <v>45</v>
-      </c>
-      <c r="I363" t="s">
-        <v>404</v>
-      </c>
-      <c r="O363" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="364" spans="1:29">
-      <c r="A364" t="s">
-        <v>407</v>
-      </c>
-      <c r="B364" t="s">
-        <v>403</v>
-      </c>
-      <c r="C364" t="s">
-        <v>27</v>
-      </c>
-      <c r="D364" t="s">
-        <v>312</v>
-      </c>
-      <c r="E364" t="s">
-        <v>29</v>
-      </c>
-      <c r="F364" t="s">
-        <v>51</v>
-      </c>
-      <c r="G364" t="s">
-        <v>31</v>
-      </c>
-      <c r="H364" t="s">
-        <v>45</v>
-      </c>
-      <c r="I364" t="s">
-        <v>404</v>
-      </c>
-      <c r="J364" t="n">
-        <v>1</v>
-      </c>
-      <c r="K364" t="n">
-        <v>4.130091911396717e-05</v>
-      </c>
-      <c r="L364" t="n">
-        <v>4.134462640193128e-05</v>
-      </c>
-      <c r="M364" t="n">
-        <v>0.1014977780216163</v>
-      </c>
-      <c r="N364" t="n">
-        <v>0.1112818261633011</v>
-      </c>
-      <c r="O364" t="n">
-        <v>2.984203395762495</v>
-      </c>
-      <c r="P364" t="n">
-        <v>2.747494668505829</v>
-      </c>
-      <c r="Q364" t="n">
-        <v>2.539529269764635</v>
-      </c>
-      <c r="R364" t="n">
-        <v>2.318261633011414</v>
-      </c>
-      <c r="S364" t="n">
-        <v>0.3022987875130301</v>
-      </c>
-      <c r="T364" t="n">
-        <v>0.3426251097453907</v>
-      </c>
-      <c r="U364" t="n">
-        <v>1</v>
-      </c>
-      <c r="V364" t="n">
-        <v>0.1014977780216163</v>
-      </c>
-      <c r="W364" t="n">
-        <v>0.1112818261633011</v>
-      </c>
-      <c r="X364" t="n">
-        <v>2.984203395762495</v>
-      </c>
-      <c r="Y364" t="n">
-        <v>2.747494668505829</v>
-      </c>
-      <c r="Z364" t="n">
-        <v>2.539529269764635</v>
-      </c>
-      <c r="AA364" t="n">
-        <v>2.318261633011414</v>
-      </c>
-      <c r="AB364" t="n">
-        <v>0.3022987875130301</v>
-      </c>
-      <c r="AC364" t="n">
-        <v>0.3426251097453907</v>
-      </c>
-    </row>
-    <row r="365" spans="1:29">
-      <c r="A365" t="s">
-        <v>408</v>
-      </c>
-      <c r="B365" t="s">
-        <v>403</v>
-      </c>
-      <c r="C365" t="s">
-        <v>27</v>
-      </c>
-      <c r="D365" t="s">
-        <v>312</v>
-      </c>
-      <c r="E365" t="s">
-        <v>29</v>
-      </c>
-      <c r="F365" t="s">
-        <v>51</v>
-      </c>
-      <c r="G365" t="s">
-        <v>31</v>
-      </c>
-      <c r="H365" t="s">
-        <v>45</v>
-      </c>
-      <c r="I365" t="s">
-        <v>404</v>
-      </c>
-      <c r="J365" t="n">
-        <v>2</v>
-      </c>
-      <c r="K365" t="n">
-        <v>4.018591629511802e-05</v>
-      </c>
-      <c r="L365" t="n">
-        <v>4.024854272479703e-05</v>
-      </c>
-      <c r="M365" t="n">
-        <v>0.1224556975914852</v>
-      </c>
-      <c r="N365" t="n">
-        <v>0.1200614574187884</v>
-      </c>
-      <c r="O365" t="n">
-        <v>2.735179920069254</v>
-      </c>
-      <c r="P365" t="n">
-        <v>2.687809438665193</v>
-      </c>
-      <c r="Q365" t="n">
-        <v>2.278707412080979</v>
-      </c>
-      <c r="R365" t="n">
-        <v>2.254170324846356</v>
-      </c>
-      <c r="S365" t="n">
-        <v>0.3622647720414769</v>
-      </c>
-      <c r="T365" t="n">
-        <v>0.353819139596137</v>
-      </c>
-      <c r="U365" t="n">
-        <v>3</v>
-      </c>
-      <c r="V365" t="n">
-        <v>0.1239370165139628</v>
-      </c>
-      <c r="W365" t="n">
-        <v>0.1239370165139628</v>
-      </c>
-      <c r="X365" t="n">
-        <v>2.698334984015215</v>
-      </c>
-      <c r="Y365" t="n">
-        <v>2.698334984015215</v>
-      </c>
-      <c r="Z365" t="n">
-        <v>2.245405168157129</v>
-      </c>
-      <c r="AA365" t="n">
-        <v>2.245405168157129</v>
-      </c>
-      <c r="AB365" t="n">
-        <v>0.366489274153728</v>
-      </c>
-      <c r="AC365" t="n">
-        <v>0.366489274153728</v>
-      </c>
-    </row>
-    <row r="366" spans="1:29">
-      <c r="A366" t="s">
-        <v>409</v>
-      </c>
-      <c r="B366" t="s">
-        <v>403</v>
-      </c>
-      <c r="C366" t="s">
-        <v>27</v>
-      </c>
-      <c r="D366" t="s">
-        <v>312</v>
-      </c>
-      <c r="E366" t="s">
-        <v>29</v>
-      </c>
-      <c r="F366" t="s">
-        <v>51</v>
-      </c>
-      <c r="G366" t="s">
-        <v>31</v>
-      </c>
-      <c r="H366" t="s">
-        <v>45</v>
-      </c>
-      <c r="I366" t="s">
-        <v>404</v>
-      </c>
-      <c r="J366" t="n">
-        <v>25</v>
-      </c>
-      <c r="K366" t="n">
-        <v>0.0007491819484906064</v>
-      </c>
-      <c r="L366" t="n">
-        <v>0.0007586044515299106</v>
-      </c>
-      <c r="M366" t="n">
-        <v>0.2416744390190377</v>
-      </c>
-      <c r="N366" t="n">
-        <v>0.2478050921861282</v>
-      </c>
-      <c r="O366" t="n">
-        <v>1.941340907920579</v>
-      </c>
-      <c r="P366" t="n">
-        <v>1.942433147381308</v>
-      </c>
-      <c r="Q366" t="n">
-        <v>1.414824161957535</v>
-      </c>
-      <c r="R366" t="n">
-        <v>1.410008779631255</v>
-      </c>
-      <c r="S366" t="n">
-        <v>0.6307675426564986</v>
-      </c>
-      <c r="T366" t="n">
-        <v>0.6305970149253731</v>
-      </c>
-      <c r="U366" t="n">
-        <v>48</v>
-      </c>
-      <c r="V366" t="n">
-        <v>0.2476545783727437</v>
-      </c>
-      <c r="W366" t="n">
-        <v>0.2423178226514486</v>
-      </c>
-      <c r="X366" t="n">
-        <v>1.920442675875217</v>
-      </c>
-      <c r="Y366" t="n">
-        <v>1.960989161087695</v>
-      </c>
-      <c r="Z366" t="n">
-        <v>1.396335107258463</v>
-      </c>
-      <c r="AA366" t="n">
-        <v>1.428007023705004</v>
-      </c>
-      <c r="AB366" t="n">
-        <v>0.635266363087727</v>
-      </c>
-      <c r="AC366" t="n">
-        <v>0.6226953467954346</v>
+        <v>0.6146924891644264</v>
       </c>
     </row>
     <row customHeight="1" ht="12.75" r="1048043" s="5" spans="1:29"/>

</xml_diff>